<commit_message>
Results from July 10, 2020 07:13:57 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-10.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-10.xlsx
@@ -522,25 +522,25 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C2" t="n">
-        <v>24459</v>
+        <v>24758</v>
       </c>
       <c r="D2" t="n">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="E2" t="n">
-        <v>2821</v>
+        <v>2851</v>
       </c>
       <c r="F2" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G2" t="n">
-        <v>0.12</v>
+        <v>11.52</v>
       </c>
       <c r="H2" t="n">
-        <v>0.13</v>
+        <v>12.82</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -569,13 +569,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C3" t="n">
-        <v>17679</v>
+        <v>18602</v>
       </c>
       <c r="D3" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -826,25 +826,25 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C8" t="n">
-        <v>18245</v>
+        <v>18670</v>
       </c>
       <c r="D8" t="n">
-        <v>612</v>
+        <v>620</v>
       </c>
       <c r="E8" t="n">
-        <v>1729</v>
+        <v>1756</v>
       </c>
       <c r="F8" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G8" t="n">
-        <v>13.88</v>
+        <v>13.57</v>
       </c>
       <c r="H8" t="n">
-        <v>15.3</v>
+        <v>15.29</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -853,10 +853,10 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>12461</v>
+        <v>12943</v>
       </c>
       <c r="L8" t="n">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="M8" t="n">
         <v>354112</v>
@@ -880,22 +880,22 @@
         <v>44022</v>
       </c>
       <c r="C9" t="n">
-        <v>26052</v>
+        <v>26803</v>
       </c>
       <c r="D9" t="n">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="E9" t="n">
-        <v>5611</v>
+        <v>5796</v>
       </c>
       <c r="F9" t="n">
         <v>74</v>
       </c>
       <c r="G9" t="n">
-        <v>24.98</v>
+        <v>25.01</v>
       </c>
       <c r="H9" t="n">
-        <v>25.52</v>
+        <v>25.26</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -904,10 +904,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>22465</v>
+        <v>23171</v>
       </c>
       <c r="L9" t="n">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="M9" t="n">
         <v>460970</v>
@@ -928,25 +928,25 @@
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C10" t="n">
-        <v>18402</v>
+        <v>18863</v>
       </c>
       <c r="D10" t="n">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="E10" t="n">
-        <v>666</v>
+        <v>690</v>
       </c>
       <c r="F10" t="n">
         <v>16</v>
       </c>
       <c r="G10" t="n">
-        <v>4.54</v>
+        <v>4.58</v>
       </c>
       <c r="H10" t="n">
-        <v>3.93</v>
+        <v>3.89</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -955,10 +955,10 @@
         <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>14668</v>
+        <v>15058</v>
       </c>
       <c r="L10" t="n">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="M10" t="n">
         <v>166412</v>
@@ -1026,20 +1026,20 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C12" t="n">
-        <v>14251</v>
+        <v>14549</v>
       </c>
       <c r="D12" t="n">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="E12" t="n">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
-        <v>1.89</v>
+        <v>1.9</v>
       </c>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="b">
@@ -1210,25 +1210,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44020</v>
+        <v>44021</v>
       </c>
       <c r="C16" t="n">
-        <v>124738</v>
+        <v>127358</v>
       </c>
       <c r="D16" t="n">
-        <v>3689</v>
+        <v>3738</v>
       </c>
       <c r="E16" t="n">
-        <v>3358</v>
+        <v>3407</v>
       </c>
       <c r="F16" t="n">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="G16" t="n">
-        <v>4.75</v>
+        <v>4.76</v>
       </c>
       <c r="H16" t="n">
-        <v>10.92</v>
+        <v>10.91</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1237,10 +1237,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>70741</v>
+        <v>71628</v>
       </c>
       <c r="L16" t="n">
-        <v>3434</v>
+        <v>3482</v>
       </c>
       <c r="M16" t="n">
         <v>823987</v>
@@ -1598,25 +1598,25 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C24" t="n">
-        <v>35525</v>
+        <v>36191</v>
       </c>
       <c r="D24" t="n">
-        <v>1706</v>
+        <v>1724</v>
       </c>
       <c r="E24" t="n">
-        <v>1854</v>
+        <v>1871</v>
       </c>
       <c r="F24" t="n">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G24" t="n">
-        <v>6.38</v>
+        <v>6.35</v>
       </c>
       <c r="H24" t="n">
-        <v>6.87</v>
+        <v>7.04</v>
       </c>
       <c r="I24" t="b">
         <v>0</v>
@@ -1625,10 +1625,10 @@
         <v>0</v>
       </c>
       <c r="K24" t="n">
-        <v>29045</v>
+        <v>29452</v>
       </c>
       <c r="L24" t="n">
-        <v>1646</v>
+        <v>1661</v>
       </c>
       <c r="M24" t="n">
         <v>227938</v>
@@ -1649,25 +1649,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C25" t="n">
-        <v>20623</v>
+        <v>20777</v>
       </c>
       <c r="D25" t="n">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="E25" t="n">
-        <v>1217</v>
+        <v>1230</v>
       </c>
       <c r="F25" t="n">
         <v>22</v>
       </c>
       <c r="G25" t="n">
-        <v>7.64</v>
+        <v>7.61</v>
       </c>
       <c r="H25" t="n">
-        <v>8.119999999999999</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="I25" t="b">
         <v>0</v>
@@ -1676,10 +1676,10 @@
         <v>1</v>
       </c>
       <c r="K25" t="n">
-        <v>15936</v>
+        <v>16169</v>
       </c>
       <c r="L25" t="n">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="M25" t="n">
         <v>90860</v>
@@ -1994,25 +1994,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C32" t="n">
-        <v>38581</v>
+        <v>39218</v>
       </c>
       <c r="D32" t="n">
-        <v>1409</v>
+        <v>1424</v>
       </c>
       <c r="E32" t="n">
-        <v>1501</v>
+        <v>1520</v>
       </c>
       <c r="F32" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G32" t="n">
-        <v>5.46</v>
+        <v>5.43</v>
       </c>
       <c r="H32" t="n">
-        <v>3.37</v>
+        <v>3.39</v>
       </c>
       <c r="I32" t="b">
         <v>0</v>
@@ -2021,10 +2021,10 @@
         <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>27467</v>
+        <v>27979</v>
       </c>
       <c r="L32" t="n">
-        <v>1336</v>
+        <v>1355</v>
       </c>
       <c r="M32" t="n">
         <v>269854</v>
@@ -2187,19 +2187,19 @@
         <v>44022</v>
       </c>
       <c r="C36" t="n">
-        <v>33931</v>
+        <v>34172</v>
       </c>
       <c r="D36" t="n">
         <v>743</v>
       </c>
       <c r="E36" t="n">
-        <v>2966</v>
+        <v>2983</v>
       </c>
       <c r="F36" t="n">
         <v>36</v>
       </c>
       <c r="G36" t="n">
-        <v>8.74</v>
+        <v>8.73</v>
       </c>
       <c r="H36" t="n">
         <v>4.85</v>
@@ -2329,25 +2329,25 @@
         </is>
       </c>
       <c r="B39" s="2" t="n">
-        <v>44021</v>
+        <v>44022</v>
       </c>
       <c r="C39" t="n">
-        <v>9428</v>
+        <v>9928</v>
       </c>
       <c r="D39" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="E39" t="n">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="F39" t="n">
         <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>1.47</v>
+        <v>1.46</v>
       </c>
       <c r="H39" t="n">
-        <v>1.02</v>
+        <v>0.99</v>
       </c>
       <c r="I39" t="b">
         <v>0</v>

</xml_diff>